<commit_message>
New design for javafx scenes
</commit_message>
<xml_diff>
--- a/EducationPlan.xlsx
+++ b/EducationPlan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>PlanID</t>
   </si>
@@ -54,6 +54,30 @@
   </si>
   <si>
     <t xml:space="preserve">balba                         </t>
+  </si>
+  <si>
+    <t>76788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info                          </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>121212</t>
+  </si>
+  <si>
+    <t>56489299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asddawsxx                     </t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -172,6 +196,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>